<commit_message>
Added Why we Sleep book in the List
</commit_message>
<xml_diff>
--- a/Venukumar_Books_List .xlsx
+++ b/Venukumar_Books_List .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Books\My Books List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EA1F2B-6CE9-4DC3-8CBD-F10E034C8C67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C79829-EB88-4757-AB75-6EEB82F7B612}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6C2F08D3-1046-4AA4-870F-D6A612D769D2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="107">
   <si>
     <t>#</t>
   </si>
@@ -327,9 +327,6 @@
     <t>George S Clason</t>
   </si>
   <si>
-    <t>Self-Developmet</t>
-  </si>
-  <si>
     <t>The Palace Of Illusions</t>
   </si>
   <si>
@@ -343,6 +340,21 @@
   </si>
   <si>
     <t>Satyanarayana Y B</t>
+  </si>
+  <si>
+    <t>80/20 Principle</t>
+  </si>
+  <si>
+    <t>Richard Koch</t>
+  </si>
+  <si>
+    <t>Why we Sleep</t>
+  </si>
+  <si>
+    <t>Mathew Walker</t>
+  </si>
+  <si>
+    <t>Health/Science</t>
   </si>
 </sst>
 </file>
@@ -780,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A302F8-F52A-450D-BD5D-7B6EE8B1BDAE}">
-  <dimension ref="E4:H56"/>
+  <dimension ref="E4:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1493,7 +1505,7 @@
         <v>96</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1501,10 +1513,10 @@
         <v>50</v>
       </c>
       <c r="F54" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G54" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>39</v>
@@ -1515,7 +1527,7 @@
         <v>51</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>26</v>
@@ -1529,13 +1541,41 @@
         <v>52</v>
       </c>
       <c r="F56" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G56" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="H56" s="4" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
+      <c r="E57" s="2">
+        <v>53</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
+      <c r="E58" s="2">
+        <v>54</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 2 more books
</commit_message>
<xml_diff>
--- a/Venukumar_Books_List .xlsx
+++ b/Venukumar_Books_List .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Books\My Books List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C79829-EB88-4757-AB75-6EEB82F7B612}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581891D2-2134-4F58-A854-5A2839595921}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6C2F08D3-1046-4AA4-870F-D6A612D769D2}"/>
   </bookViews>
@@ -23,18 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="109">
   <si>
     <t>#</t>
   </si>
@@ -355,6 +349,12 @@
   </si>
   <si>
     <t>Health/Science</t>
+  </si>
+  <si>
+    <t>Outwitting the Devil</t>
+  </si>
+  <si>
+    <t>The Oaths of Vayuputras - Shiva trilogy book-3</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -471,6 +471,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -792,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A302F8-F52A-450D-BD5D-7B6EE8B1BDAE}">
-  <dimension ref="E4:H58"/>
+  <dimension ref="E4:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L57" sqref="L57"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1578,6 +1590,40 @@
         <v>106</v>
       </c>
     </row>
+    <row r="59" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
+      <c r="E59" s="2">
+        <v>55</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
+      <c r="E60" s="2">
+        <v>56</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
+      <c r="E61" s="8"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding 5 More Books to the List
</commit_message>
<xml_diff>
--- a/Venukumar_Books_List .xlsx
+++ b/Venukumar_Books_List .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Books\My Books List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581891D2-2134-4F58-A854-5A2839595921}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44115E20-F6C0-425A-9636-4903236C97EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6C2F08D3-1046-4AA4-870F-D6A612D769D2}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="119">
   <si>
     <t>#</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Kanled Hosseini</t>
   </si>
   <si>
-    <t>Think And Grow Rich</t>
-  </si>
-  <si>
     <t>Napolean Hill</t>
   </si>
   <si>
@@ -355,6 +352,39 @@
   </si>
   <si>
     <t>The Oaths of Vayuputras - Shiva trilogy book-3</t>
+  </si>
+  <si>
+    <t>Think And Grow Rich - Read Twice</t>
+  </si>
+  <si>
+    <t>When All Is Not Well</t>
+  </si>
+  <si>
+    <t>Om Swami</t>
+  </si>
+  <si>
+    <t>Spiritual - Self help</t>
+  </si>
+  <si>
+    <t>Mind full to Mindful</t>
+  </si>
+  <si>
+    <t>Quite</t>
+  </si>
+  <si>
+    <t>Susan Cain</t>
+  </si>
+  <si>
+    <t>Awaken The Giant Within</t>
+  </si>
+  <si>
+    <t>Anthony Robbinson</t>
+  </si>
+  <si>
+    <t>Deep Work</t>
+  </si>
+  <si>
+    <t>Cal Newport</t>
   </si>
 </sst>
 </file>
@@ -452,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -473,16 +503,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -804,16 +825,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A302F8-F52A-450D-BD5D-7B6EE8B1BDAE}">
-  <dimension ref="E4:H61"/>
+  <dimension ref="E4:H66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+      <selection activeCell="L59" sqref="L59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="9.140625" style="5"/>
-    <col min="5" max="5" width="4.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="60" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.42578125" style="6" bestFit="1" customWidth="1"/>
@@ -1007,10 +1028,10 @@
         <v>13</v>
       </c>
       <c r="F17" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>11</v>
@@ -1021,10 +1042,10 @@
         <v>14</v>
       </c>
       <c r="F18" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>7</v>
@@ -1035,10 +1056,10 @@
         <v>15</v>
       </c>
       <c r="F19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>11</v>
@@ -1049,13 +1070,13 @@
         <v>16</v>
       </c>
       <c r="F20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1063,10 +1084,10 @@
         <v>17</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>7</v>
@@ -1077,10 +1098,10 @@
         <v>18</v>
       </c>
       <c r="F22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>7</v>
@@ -1091,7 +1112,7 @@
         <v>19</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>10</v>
@@ -1105,7 +1126,7 @@
         <v>20</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>26</v>
@@ -1119,10 +1140,10 @@
         <v>21</v>
       </c>
       <c r="F25" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>11</v>
@@ -1133,10 +1154,10 @@
         <v>22</v>
       </c>
       <c r="F26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>11</v>
@@ -1147,13 +1168,13 @@
         <v>23</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="28" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1161,10 +1182,10 @@
         <v>24</v>
       </c>
       <c r="F28" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>11</v>
@@ -1175,13 +1196,13 @@
         <v>25</v>
       </c>
       <c r="F29" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="H29" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="30" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1189,13 +1210,13 @@
         <v>26</v>
       </c>
       <c r="F30" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="H30" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1203,7 +1224,7 @@
         <v>27</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>22</v>
@@ -1217,10 +1238,10 @@
         <v>28</v>
       </c>
       <c r="F32" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>11</v>
@@ -1231,7 +1252,7 @@
         <v>29</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>30</v>
@@ -1245,10 +1266,10 @@
         <v>30</v>
       </c>
       <c r="F34" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>11</v>
@@ -1259,10 +1280,10 @@
         <v>31</v>
       </c>
       <c r="F35" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>11</v>
@@ -1273,10 +1294,10 @@
         <v>32</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>11</v>
@@ -1287,10 +1308,10 @@
         <v>33</v>
       </c>
       <c r="F37" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>11</v>
@@ -1301,13 +1322,13 @@
         <v>34</v>
       </c>
       <c r="F38" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="H38" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="39" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1315,10 +1336,10 @@
         <v>35</v>
       </c>
       <c r="F39" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>11</v>
@@ -1329,10 +1350,10 @@
         <v>36</v>
       </c>
       <c r="F40" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>11</v>
@@ -1343,13 +1364,13 @@
         <v>37</v>
       </c>
       <c r="F41" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="H41" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="42" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1357,10 +1378,10 @@
         <v>38</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>11</v>
@@ -1371,7 +1392,7 @@
         <v>39</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>10</v>
@@ -1385,10 +1406,10 @@
         <v>40</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>11</v>
@@ -1399,13 +1420,13 @@
         <v>41</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1413,10 +1434,10 @@
         <v>42</v>
       </c>
       <c r="F46" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>11</v>
@@ -1427,10 +1448,10 @@
         <v>43</v>
       </c>
       <c r="F47" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G47" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>11</v>
@@ -1441,13 +1462,13 @@
         <v>44</v>
       </c>
       <c r="F48" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="G48" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="H48" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1455,10 +1476,10 @@
         <v>45</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>11</v>
@@ -1469,10 +1490,10 @@
         <v>46</v>
       </c>
       <c r="F50" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>11</v>
@@ -1483,10 +1504,10 @@
         <v>47</v>
       </c>
       <c r="F51" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>11</v>
@@ -1497,10 +1518,10 @@
         <v>48</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>11</v>
@@ -1511,10 +1532,10 @@
         <v>49</v>
       </c>
       <c r="F53" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G53" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>11</v>
@@ -1525,13 +1546,13 @@
         <v>50</v>
       </c>
       <c r="F54" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G54" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G54" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="H54" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1539,7 +1560,7 @@
         <v>51</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>26</v>
@@ -1553,10 +1574,10 @@
         <v>52</v>
       </c>
       <c r="F56" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G56" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="H56" s="4" t="s">
         <v>14</v>
@@ -1567,10 +1588,10 @@
         <v>53</v>
       </c>
       <c r="F57" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G57" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="H57" s="4" t="s">
         <v>11</v>
@@ -1581,13 +1602,13 @@
         <v>54</v>
       </c>
       <c r="F58" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G58" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G58" s="3" t="s">
+      <c r="H58" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="59" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1595,10 +1616,10 @@
         <v>55</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>11</v>
@@ -1609,20 +1630,90 @@
         <v>56</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G60" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H60" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H60" s="4" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="61" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
-      <c r="E61" s="8"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="10"/>
-      <c r="H61" s="11"/>
+      <c r="E61" s="2">
+        <v>57</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
+      <c r="E62" s="2">
+        <v>58</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="63" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
+      <c r="E63" s="8">
+        <v>59</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
+      <c r="E64" s="2">
+        <v>60</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
+      <c r="E65" s="2">
+        <v>61</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added 2 books to the list
</commit_message>
<xml_diff>
--- a/Venukumar_Books_List .xlsx
+++ b/Venukumar_Books_List .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Books\My Books List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44115E20-F6C0-425A-9636-4903236C97EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C911B4-382F-4623-B1FC-ECDCFB48FD32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6C2F08D3-1046-4AA4-870F-D6A612D769D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6C2F08D3-1046-4AA4-870F-D6A612D769D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="124">
   <si>
     <t>#</t>
   </si>
@@ -385,6 +385,21 @@
   </si>
   <si>
     <t>Cal Newport</t>
+  </si>
+  <si>
+    <t>Solitaire</t>
+  </si>
+  <si>
+    <t>Alice oslem</t>
+  </si>
+  <si>
+    <t>The Silva - Mind controlling techniques</t>
+  </si>
+  <si>
+    <t>Jose Silva</t>
+  </si>
+  <si>
+    <t>Self-Decvelopment</t>
   </si>
 </sst>
 </file>
@@ -825,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A302F8-F52A-450D-BD5D-7B6EE8B1BDAE}">
-  <dimension ref="E4:H66"/>
+  <dimension ref="E4:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L59" sqref="L59"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1709,11 +1724,39 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
+    <row r="66" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
+      <c r="E66" s="2">
+        <v>62</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
+      <c r="E67" s="2">
+        <v>63</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>